<commit_message>
feat: add new financial evaluation files and update existing evaluation criteria
</commit_message>
<xml_diff>
--- a/public/종합_평가지표_스코어링_최종_변수명포함.xlsx
+++ b/public/종합_평가지표_스코어링_최종_변수명포함.xlsx
@@ -1,20 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\potatoinvest\public\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135FE010-CF8B-481A-B718-F93E0F90C507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="평가" sheetId="1" r:id="rId1"/>
+    <sheet name="배당" sheetId="2" r:id="rId2"/>
+    <sheet name="수익성" sheetId="3" r:id="rId3"/>
+    <sheet name="손익계산" sheetId="4" r:id="rId4"/>
+    <sheet name="대차대조표" sheetId="5" r:id="rId5"/>
+    <sheet name="현금흐름" sheetId="6" r:id="rId6"/>
+    <sheet name="테크니컬즈" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="250">
   <si>
     <t>라벨</t>
   </si>
@@ -389,17 +401,913 @@
   </si>
   <si>
     <t>EBITDA 대비 매우 저평가 상태입니다. 적극 매수를 고려해야 합니다.</t>
+  </si>
+  <si>
+    <t>배당 수익</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>배당 비율</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DPS 성장</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>주당 배당금 증가율 %</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>배당 성향 %</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>배당 수익률 %</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>연속 배당 지불</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지속적인 배당금 지급</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>연속 배당 성장</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지속적인 배당금 증가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>총마진</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>총마진%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>영업마진</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>영업마진%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>세전마진%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>세전 마진</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FCF 마진</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>잉여 현금 흐름 마진 %</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ROA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ROE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>총자산 이익률 %</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자기자본 수익률 %</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>투하자본 수익률</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>투하자본 수익률 %</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R&amp;D 비율</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>연구 개발 비율 %</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>판관비율</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>판매, 일반 및 관리 비용 비율</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>매출 성장률</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>매출 성장률 %</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EPS 희석 성장</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>희석 주당순이익 성장률 %</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>유동비율</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>당좌비율</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>부채 / 자본</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>부채 비율</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>현금 / 부채</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>현금 대비 부채 비율</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기술등급</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MA 레이팅</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Os 등급</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mom</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>스토캐스틱 %K</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>스토캐스틱 %D</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>커모디티 채널 인덱스</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>오썸 오실레이터</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>모멘텀</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상대강도지수</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>오실레이터 레이팅</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>무빙 애버리지 레이팅</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>테크니컬 레이팅</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dividends_yield_current</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dividend_payout_ratio_ttm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dps_common_stock_prim_issue_yoy_growth_fy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>continuous_dividend_payout</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>continuous_dividend_growth</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>7~10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3~7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1~3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt; 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">배당수익률이 너무 높습니다. 배당 삭감 위험이나 주가 하락을 의심해봐야 합니다. 신중한 검토가 필요해요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🚨</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">높은 배당수익률이지만 지속가능성을 확인해야 합니다. 회사 재무상태를 꼼꼼히 살펴보세요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>⚠️</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">적정한 배당수익률입니다. 안정적인 배당 투자에 적합한 수준이에요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">낮지만 안전한 배당수익률입니다. 성장주 성격이 강할 수 있어요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">배당수익률이 매우 낮습니다. 배당보다는 성장에 집중하는 회사일 가능성이 높아요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>📈</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 100</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>80~100</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>40~80</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>20~40</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt; 20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">이익보다 더 많은 배당을 지급하고 있어요. 배당 삭감 위험이 매우 높습니다 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🚨</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">이익의 대부분을 배당으로 지급하고 있어요. 성장 투자 여력이 부족할 수 있습니다 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>⚠️</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">적정한 수준의 배당성향입니다. 배당과 성장의 균형이 잘 맞아요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">보수적인 배당정책을 펼치고 있어요. 미래 배당 증가 여력이 충분합니다 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">배당보다는 성장에 집중하는 회사예요. 배당수익률은 낮을 수 있어요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>📈</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>-50~-10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt; -50</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>-10~30</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>30~100</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">배당금이 크게 삭감되었어요. 회사 상황이 어려울 수 있습니다 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😰</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">배당금이 감소했어요. 회사의 재무상태를 확인해봐야 합니다 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>⚠️</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">안정적인 배당금 증가율이에요. 꾸준한 배당 성장을 기대할 수 있어요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">좋은 배당금 증가율이에요! 배당 투자자에게 매력적인 수준입니다 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🚀</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">배당금이 너무 급격히 증가했어요. 일회성일 가능성이 높으니 주의하세요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤔</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0~2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3~5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6~10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>11~15</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 15</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">배당 이력이 짧아요. 아직 배당 정책이 안정화되지 않았을 수 있어요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤷‍♂️</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">배당 이력이 비교적 짧아요. 배당의 지속성을 좀 더 지켜봐야겠어요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤔</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">적당한 배당 이력을 가지고 있어요. 어느 정도 신뢰할 수 있는 수준이에요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오랫동안 꾸준히 배당을 지급해왔어요. 안정적인 배당주로 볼 수 있어요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">매우 오랜 기간 배당을 유지해온 우량 배당주예요! 신뢰도가 매우 높습니다 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>💎</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">배당 증가 이력이 짧아요. 앞으로의 배당 증가를 지켜봐야겠어요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🌱</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">몇 년간 배당을 늘려왔어요. 이 추세가 계속될지 관심을 가져보세요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>📈</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">꾸준히 배당을 늘려온 회사예요. 배당 성장주로서 매력이 있어요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오랫동안 배당을 지속적으로 늘려왔어요. 훌륭한 배당 성장주입니다 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🚀</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">배당킹(Dividend King) 수준이에요! 최고급 배당 성장주로 인정받는 기업입니다 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👑</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gross_margin_ttm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt; 0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0~20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>40~60</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 60</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">총마진이 음수예요. 원가가 매출보다 높아 매우 위험한 상황입니다 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😰</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">총마진이 낮아요. 원가 관리나 가격 정책을 개선할 필요가 있어 보여요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😕</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">적정한 총마진이에요. 기본적인 수익성은 확보하고 있어요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">좋은 총마진이에요! 제품/서비스의 경쟁력이 우수합니다 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">매우 높은 총마진이에요! 강력한 경쟁우위를 가진 사업모델입니다 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🚀</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>operating_margin_ttm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0~5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5~15</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>15~25</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 25</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">영업적자 상태예요. 사업 구조 개선이 시급합니다 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😰</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">영업마진이 낮아요. 운영 효율성을 높일 필요가 있어요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😕</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">적당한 영업마진이에요. 기본적인 사업성은 확보했어요 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">좋은 영업마진이에요! 효율적인 운영을 하고 있습니다 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">매우 높은 영업마진이에요! 탁월한 운영 효율성을 보여줍니다 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🚀</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">세전손실 상태예요. 전반적인 수익성 개선이 필요합니다 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😰</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pre_tax_margin_ttm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -407,9 +1315,28 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI Symbol"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI Emoji"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -447,24 +1374,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -502,7 +1441,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -536,6 +1475,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -570,9 +1510,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -745,14 +1686,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -799,7 +1747,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -813,7 +1761,7 @@
         <v>4.08</v>
       </c>
       <c r="E2">
-        <v>662.8200000000001</v>
+        <v>662.82</v>
       </c>
       <c r="F2" t="s">
         <v>43</v>
@@ -846,7 +1794,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -857,10 +1805,10 @@
         <v>36</v>
       </c>
       <c r="D3">
-        <v>-0.58</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="E3">
-        <v>272.04</v>
+        <v>272.04000000000002</v>
       </c>
       <c r="F3" t="s">
         <v>44</v>
@@ -893,7 +1841,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -940,7 +1888,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -987,7 +1935,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1001,7 +1949,7 @@
         <v>1.56</v>
       </c>
       <c r="E6">
-        <v>290.35</v>
+        <v>290.35000000000002</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
@@ -1034,7 +1982,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1081,7 +2029,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1128,7 +2076,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1175,7 +2123,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1222,7 +2170,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1233,7 +2181,7 @@
         <v>24</v>
       </c>
       <c r="D11">
-        <v>2.03</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="E11">
         <v>1531.4</v>
@@ -1270,6 +2218,1126 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0FC1E3-BB82-4C09-AAB1-EADE583864FE}">
+  <dimension ref="A1:O6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>9.86</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-22146.34</v>
+      </c>
+      <c r="E3" s="3">
+        <v>699.83</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="3">
+        <v>-100</v>
+      </c>
+      <c r="E4" s="3">
+        <v>450</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>19</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD74B407-206A-4DD1-95CB-CF7DC0760063}">
+  <dimension ref="A1:O10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.875" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="3">
+        <v>-250881.6</v>
+      </c>
+      <c r="E2" s="3">
+        <v>411.28</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-1360291.24</v>
+      </c>
+      <c r="E3" s="3">
+        <v>22789.47</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="3">
+        <v>-6081785.71</v>
+      </c>
+      <c r="E4" s="3">
+        <v>861486.5</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="3">
+        <v>-8548516.5999999996</v>
+      </c>
+      <c r="E5" s="3">
+        <v>262044.95</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="3">
+        <v>328501.01</v>
+      </c>
+      <c r="E6" s="3">
+        <v>64408.24</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="3">
+        <v>-60832.47</v>
+      </c>
+      <c r="E7" s="3">
+        <v>12062.12</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="3">
+        <v>-22746.15</v>
+      </c>
+      <c r="E8" s="3">
+        <v>12062.12</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" s="3">
+        <v>-222.45</v>
+      </c>
+      <c r="E9" s="3">
+        <v>670130.43000000005</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D10" s="3">
+        <v>-826.24</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1333595.24</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC4A9AC-4ECE-4E24-B357-0067097A5105}">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2">
+        <v>-31613.21</v>
+      </c>
+      <c r="E2">
+        <v>2814518.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3">
+        <v>-235900</v>
+      </c>
+      <c r="E3">
+        <v>45688.57</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AACBD2-4903-47AA-86A7-49EF29DEA89C}">
+  <dimension ref="A1:O5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>22355</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>22355</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>385.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>18613.57</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DCAAA7E-B440-4D9D-BC53-DF0BECCFA49C}">
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E16:E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C233B90-99E2-480E-87B0-55CA836C52DA}">
+  <dimension ref="A1:O10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="E15:F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D5">
+        <v>6.16</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6">
+        <v>-5414.8</v>
+      </c>
+      <c r="E6">
+        <v>14200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7">
+        <v>-147411.75260000001</v>
+      </c>
+      <c r="E7">
+        <v>12308.59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D8">
+        <v>-666.67</v>
+      </c>
+      <c r="E8">
+        <v>666.67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C10" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>